<commit_message>
Correction LFI > FI
</commit_message>
<xml_diff>
--- a/données externes/affiliation_elections.xlsx
+++ b/données externes/affiliation_elections.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura\OneDrive\Bureau\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laura\OneDrive\Documents\MS BDAAD\Tweets Project\Twitter_Elections_Repo\Twitter-Elections\données externes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{3E083759-3C13-4582-9877-7EB90BECA1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5C152F9-652B-4F7E-9C55-70B18AB01FC1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D448C61-19FE-4E8E-B587-C7F9F215C189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DDA95EC5-36B9-4442-BC5D-EB247E477A5F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="31">
   <si>
     <t>id</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>REC</t>
-  </si>
-  <si>
-    <t>LFI</t>
   </si>
   <si>
     <t>ECO</t>
@@ -137,7 +134,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,7 +196,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -498,18 +495,18 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11</v>
       </c>
@@ -564,7 +561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>12</v>
       </c>
@@ -590,7 +587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>13</v>
       </c>
@@ -616,7 +613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>14</v>
       </c>
@@ -642,7 +639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>15</v>
       </c>
@@ -668,7 +665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>16</v>
       </c>
@@ -694,7 +691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>17</v>
       </c>
@@ -720,7 +717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>18</v>
       </c>
@@ -731,7 +728,7 @@
         <v>2022</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E9">
         <v>75</v>
@@ -746,7 +743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>19</v>
       </c>
@@ -757,7 +754,7 @@
         <v>2022</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10">
         <v>75</v>
@@ -772,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>20</v>
       </c>
@@ -783,7 +780,7 @@
         <v>2017</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11">
         <v>75</v>
@@ -801,7 +798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>21</v>
       </c>
@@ -830,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>22</v>
       </c>
@@ -841,7 +838,7 @@
         <v>2017</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13">
         <v>75</v>
@@ -859,7 +856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>23</v>
       </c>
@@ -870,7 +867,7 @@
         <v>2017</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14">
         <v>75</v>
@@ -888,7 +885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>24</v>
       </c>
@@ -899,7 +896,7 @@
         <v>2017</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15">
         <v>75</v>
@@ -917,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>25</v>
       </c>
@@ -928,7 +925,7 @@
         <v>2017</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16">
         <v>75</v>
@@ -946,7 +943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>26</v>
       </c>
@@ -957,7 +954,7 @@
         <v>2017</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E17">
         <v>75</v>
@@ -975,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>27</v>
       </c>
@@ -1004,7 +1001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>28</v>
       </c>
@@ -1033,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>29</v>
       </c>
@@ -1062,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>30</v>
       </c>
@@ -1091,7 +1088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>31</v>
       </c>
@@ -1102,7 +1099,7 @@
         <v>2017</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E22">
         <v>75</v>
@@ -1120,7 +1117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>32</v>
       </c>
@@ -1149,7 +1146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>33</v>
       </c>
@@ -1160,7 +1157,7 @@
         <v>2017</v>
       </c>
       <c r="D24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E24">
         <v>75</v>
@@ -1178,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>34</v>
       </c>
@@ -1189,7 +1186,7 @@
         <v>2017</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E25">
         <v>75</v>
@@ -1207,7 +1204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>35</v>
       </c>
@@ -1218,7 +1215,7 @@
         <v>2017</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E26">
         <v>75</v>
@@ -1236,7 +1233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>36</v>
       </c>
@@ -1265,7 +1262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>37</v>
       </c>
@@ -1276,7 +1273,7 @@
         <v>2017</v>
       </c>
       <c r="D28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E28">
         <v>75</v>
@@ -1294,7 +1291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>38</v>
       </c>
@@ -1305,7 +1302,7 @@
         <v>2017</v>
       </c>
       <c r="D29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E29">
         <v>75</v>
@@ -1323,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>39</v>
       </c>
@@ -1352,7 +1349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>40</v>
       </c>
@@ -1381,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>41</v>
       </c>
@@ -1392,7 +1389,7 @@
         <v>2012</v>
       </c>
       <c r="D32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E32">
         <v>75</v>
@@ -1410,7 +1407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>42</v>
       </c>
@@ -1439,7 +1436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>43</v>
       </c>
@@ -1450,7 +1447,7 @@
         <v>2012</v>
       </c>
       <c r="D34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E34">
         <v>75</v>
@@ -1468,7 +1465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>44</v>
       </c>
@@ -1479,7 +1476,7 @@
         <v>2012</v>
       </c>
       <c r="D35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E35">
         <v>75</v>
@@ -1497,7 +1494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>45</v>
       </c>
@@ -1508,7 +1505,7 @@
         <v>2012</v>
       </c>
       <c r="D36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E36">
         <v>75</v>
@@ -1526,7 +1523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>46</v>
       </c>
@@ -1555,7 +1552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>47</v>
       </c>
@@ -1566,7 +1563,7 @@
         <v>2012</v>
       </c>
       <c r="D38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E38">
         <v>75</v>
@@ -1584,7 +1581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>48</v>
       </c>
@@ -1595,7 +1592,7 @@
         <v>2012</v>
       </c>
       <c r="D39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E39">
         <v>75</v>
@@ -1613,7 +1610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>49</v>
       </c>
@@ -1624,7 +1621,7 @@
         <v>2012</v>
       </c>
       <c r="D40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E40">
         <v>75</v>
@@ -1642,7 +1639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>50</v>
       </c>
@@ -1653,7 +1650,7 @@
         <v>2012</v>
       </c>
       <c r="D41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E41">
         <v>75</v>
@@ -1671,7 +1668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>51</v>
       </c>
@@ -1700,7 +1697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>52</v>
       </c>
@@ -1711,7 +1708,7 @@
         <v>2012</v>
       </c>
       <c r="D43" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E43">
         <v>75</v>
@@ -1729,7 +1726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>53</v>
       </c>
@@ -1740,7 +1737,7 @@
         <v>2012</v>
       </c>
       <c r="D44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E44">
         <v>75</v>
@@ -1758,7 +1755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>54</v>
       </c>
@@ -1769,7 +1766,7 @@
         <v>2012</v>
       </c>
       <c r="D45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E45">
         <v>75</v>
@@ -1787,7 +1784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>55</v>
       </c>
@@ -1798,7 +1795,7 @@
         <v>2012</v>
       </c>
       <c r="D46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E46">
         <v>75</v>
@@ -1823,25 +1820,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bff903b3-f4d0-413f-a493-3d323afbaa16">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009B502737A4FCC24B970DDDE816F64481" ma:contentTypeVersion="9" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="59a0a30de368131caad882c61bef2b51">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bff903b3-f4d0-413f-a493-3d323afbaa16" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e610a3daa0bc582e9b4ecf71207f5cef" ns2:_="">
     <xsd:import namespace="bff903b3-f4d0-413f-a493-3d323afbaa16"/>
@@ -2015,14 +1993,57 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bff903b3-f4d0-413f-a493-3d323afbaa16">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{602C1CCF-8C9E-42AF-88E7-9D8DD6AF5DE7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{558093E7-3810-4E0A-B5A1-A9AA2C2C967F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bff903b3-f4d0-413f-a493-3d323afbaa16"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86662311-447F-49EF-AD9F-382AEDE6177C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86662311-447F-49EF-AD9F-382AEDE6177C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bff903b3-f4d0-413f-a493-3d323afbaa16"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{558093E7-3810-4E0A-B5A1-A9AA2C2C967F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{602C1CCF-8C9E-42AF-88E7-9D8DD6AF5DE7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>